<commit_message>
format csv update; soundscape clusters 1 and 2 supported
</commit_message>
<xml_diff>
--- a/csv_format.xlsx
+++ b/csv_format.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eliu\Documents\2022_Spring\Classes\CPSC432_ComputerMusic\final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alvin\Desktop\Synesthesis_Liu_Shi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255275F7-FB47-4A15-B23E-A55016A4C84B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F4D831-A15D-4568-AC32-1E3EA45FA20A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{8A07288D-0CE9-4B50-A3AC-B530B2072068}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{8A07288D-0CE9-4B50-A3AC-B530B2072068}"/>
   </bookViews>
   <sheets>
     <sheet name="csv_1" sheetId="1" r:id="rId1"/>
@@ -432,12 +432,12 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -466,19 +466,100 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>6</v>
+      </c>
+      <c r="H2">
+        <v>7</v>
+      </c>
+      <c r="I2">
+        <v>8</v>
+      </c>
+      <c r="J2">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+      <c r="J3">
+        <v>9</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>6</v>
+      </c>
+      <c r="H4">
+        <v>7</v>
+      </c>
+      <c r="I4">
+        <v>8</v>
+      </c>
+      <c r="J4">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -494,14 +575,14 @@
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>

</xml_diff>